<commit_message>
Updated progress for 'Real Numbers and Real Analysis'
</commit_message>
<xml_diff>
--- a/Progress Trackers/Rudin - Principles of Mathematical Analysis.xlsx
+++ b/Progress Trackers/Rudin - Principles of Mathematical Analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeX\Books\Repository\Progress Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E50E77-A6AD-40D8-AAD1-9407C2EF37EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C11B6B9-E00C-4B0C-AEFF-8EDB530D6D16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0465A5A-47AB-481B-AF62-12180F11677C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
   <si>
     <t>Done</t>
   </si>
@@ -429,7 +429,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,6 +527,9 @@
       <c r="H2" s="1">
         <v>1</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="J2" s="1">
         <v>1</v>
       </c>
@@ -1746,7 +1749,7 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2">
-        <f t="shared" ref="D34:W34" si="12">E$1</f>
+        <f t="shared" ref="E34:W34" si="12">E$1</f>
         <v>2</v>
       </c>
       <c r="F34" s="2"/>
@@ -1804,7 +1807,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" ref="D35:W35" si="13">COUNTIF(E$2:E$33,"Done")</f>
+        <f t="shared" ref="E35:W35" si="13">COUNTIF(E$2:E$33,"Done")</f>
         <v>2</v>
       </c>
       <c r="G35" s="3">
@@ -1813,7 +1816,7 @@
       </c>
       <c r="I35" s="3">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K35" s="3">
         <f t="shared" si="13"/>
@@ -1848,7 +1851,7 @@
       </c>
       <c r="Y35" s="3">
         <f>SUM(C35:W35)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1860,7 +1863,7 @@
         <v>20</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" ref="D36:W36" si="14">COUNT(D$2:D$33)</f>
+        <f t="shared" ref="E36:W36" si="14">COUNT(D$2:D$33)</f>
         <v>30</v>
       </c>
       <c r="G36" s="3">
@@ -1916,7 +1919,7 @@
         <v>0.3</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" ref="D37:W37" si="15">E35/E36</f>
+        <f t="shared" ref="E37:W37" si="15">E35/E36</f>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="G37" s="4">
@@ -1925,7 +1928,7 @@
       </c>
       <c r="I37" s="4">
         <f t="shared" si="15"/>
-        <v>3.8461538461538464E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="K37" s="4">
         <f t="shared" si="15"/>
@@ -1960,7 +1963,7 @@
       </c>
       <c r="Y37" s="4">
         <f>Y35/Y36</f>
-        <v>3.8327526132404179E-2</v>
+        <v>4.1811846689895474E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>